<commit_message>
binder data likely not enough
</commit_message>
<xml_diff>
--- a/dy_binding_data.xlsx
+++ b/dy_binding_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="2300" windowWidth="18780" windowHeight="12060" tabRatio="500"/>
+    <workbookView xWindow="440" yWindow="2980" windowWidth="23060" windowHeight="12060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="dy_binding_data.csv" sheetId="1" r:id="rId1"/>
@@ -3421,8 +3421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q986"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A653" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3517,6 +3517,10 @@
       <c r="O2">
         <v>5.9117832000000002E-2</v>
       </c>
+      <c r="P2">
+        <f>C2+D2+E2+F2+G2+H2</f>
+        <v>1.0000000010000001</v>
+      </c>
       <c r="Q2" t="s">
         <v>15</v>
       </c>
@@ -3567,6 +3571,10 @@
       <c r="O3">
         <v>-0.45027624300000002</v>
       </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P66" si="0">C3+D3+E3+F3+G3+H3</f>
+        <v>1</v>
+      </c>
       <c r="Q3" t="s">
         <v>18</v>
       </c>
@@ -3617,6 +3625,10 @@
       <c r="O4">
         <v>-0.309726157</v>
       </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>0.99999999900000003</v>
+      </c>
       <c r="Q4" t="s">
         <v>21</v>
       </c>
@@ -3667,6 +3679,10 @@
       <c r="O5">
         <v>0.72535211300000002</v>
       </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999989</v>
+      </c>
       <c r="Q5" t="s">
         <v>24</v>
       </c>
@@ -3717,6 +3733,10 @@
       <c r="O6">
         <v>-3.3519553000000001E-2</v>
       </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="Q6" t="s">
         <v>27</v>
       </c>
@@ -3767,6 +3787,10 @@
       <c r="O7">
         <v>-0.93589743599999997</v>
       </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>1.0000000010000001</v>
+      </c>
       <c r="Q7" t="s">
         <v>30</v>
       </c>
@@ -3817,6 +3841,10 @@
       <c r="O8">
         <v>-1.5384615000000001E-2</v>
       </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -3864,6 +3892,10 @@
       <c r="O9">
         <v>-0.81355932200000003</v>
       </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -3911,6 +3943,10 @@
       <c r="O10">
         <v>0.743243243</v>
       </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>1.0000000010000001</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -3958,6 +3994,10 @@
       <c r="O11">
         <v>0.256578947</v>
       </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -4005,6 +4045,10 @@
       <c r="O12">
         <v>0.304560261</v>
       </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>0.99999999800000006</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -4052,6 +4096,10 @@
       <c r="O13">
         <v>-0.29675810499999999</v>
       </c>
+      <c r="P13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -4099,6 +4147,10 @@
       <c r="O14">
         <v>0.88034188000000002</v>
       </c>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -4146,6 +4198,10 @@
       <c r="O15">
         <v>7.1835804000000003E-2</v>
       </c>
+      <c r="P15">
+        <f t="shared" si="0"/>
+        <v>0.99999999900000003</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -4193,8 +4249,12 @@
       <c r="O16">
         <v>0.88794567099999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P16">
+        <f t="shared" si="0"/>
+        <v>0.99999999900000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -4240,8 +4300,12 @@
       <c r="O17">
         <v>-0.87912087900000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P17">
+        <f t="shared" si="0"/>
+        <v>0.99999999900000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -4287,8 +4351,12 @@
       <c r="O18">
         <v>0.40243902399999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -4334,8 +4402,12 @@
       <c r="O19">
         <v>0.47641509399999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -4381,8 +4453,12 @@
       <c r="O20">
         <v>0.18478260899999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P20">
+        <f>C20+D20+E20+F20+G20+H20</f>
+        <v>0.99999999900000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -4428,8 +4504,12 @@
       <c r="O21">
         <v>-0.89423076899999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -4475,8 +4555,12 @@
       <c r="O22">
         <v>-4.0280209999999997E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P22">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -4522,8 +4606,12 @@
       <c r="O23">
         <v>0.85714285700000004</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P23">
+        <f t="shared" si="0"/>
+        <v>1.0000000009999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -4569,8 +4657,12 @@
       <c r="O24">
         <v>0.156494523</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -4616,8 +4708,12 @@
       <c r="O25">
         <v>0.10820700499999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -4663,8 +4759,12 @@
       <c r="O26">
         <v>-0.31753554499999997</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P26">
+        <f t="shared" si="0"/>
+        <v>0.99999999900000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -4710,8 +4810,12 @@
       <c r="O27">
         <v>0.42168674699999997</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P27">
+        <f t="shared" si="0"/>
+        <v>1.0000000010000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -4757,8 +4861,12 @@
       <c r="O28">
         <v>-0.18181818199999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P28">
+        <f t="shared" si="0"/>
+        <v>1.0000000009999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -4804,8 +4912,12 @@
       <c r="O29">
         <v>0.41428571400000003</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P29">
+        <f t="shared" si="0"/>
+        <v>1.0000000010000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -4851,8 +4963,12 @@
       <c r="O30">
         <v>-3.8976856999999997E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -4898,8 +5014,12 @@
       <c r="O31">
         <v>0.32129032299999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P31">
+        <f t="shared" si="0"/>
+        <v>1.0000000010000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -4945,8 +5065,12 @@
       <c r="O32">
         <v>0.36971046800000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P32">
+        <f t="shared" si="0"/>
+        <v>0.99999999900000014</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -4992,8 +5116,12 @@
       <c r="O33">
         <v>-0.18390804599999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -5039,8 +5167,12 @@
       <c r="O34">
         <v>0.35640413700000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P34">
+        <f t="shared" si="0"/>
+        <v>0.99999999900000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -5086,8 +5218,12 @@
       <c r="O35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
@@ -5133,8 +5269,12 @@
       <c r="O36">
         <v>-0.244897959</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P36">
+        <f>C36+D36+E36+F36+G36+H36</f>
+        <v>1.0000000010000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -5180,8 +5320,12 @@
       <c r="O37">
         <v>-0.83088235300000002</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P37">
+        <f t="shared" si="0"/>
+        <v>1.0000000019999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
@@ -5227,8 +5371,12 @@
       <c r="O38">
         <v>-0.608058608</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
@@ -5274,8 +5422,12 @@
       <c r="O39">
         <v>1.3353116E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P39">
+        <f t="shared" si="0"/>
+        <v>0.99999999899999992</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
@@ -5321,8 +5473,12 @@
       <c r="O40">
         <v>0.94949494899999998</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P40">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
@@ -5368,8 +5524,12 @@
       <c r="O41">
         <v>0.11627907</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P41">
+        <f t="shared" si="0"/>
+        <v>0.99999999899999992</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -5415,8 +5575,12 @@
       <c r="O42">
         <v>0.14272685800000001</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P42">
+        <f t="shared" si="0"/>
+        <v>0.99999999900000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
@@ -5462,8 +5626,12 @@
       <c r="O43">
         <v>-0.88135593199999995</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P43">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
@@ -5509,8 +5677,12 @@
       <c r="O44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P44">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
@@ -5556,8 +5728,12 @@
       <c r="O45">
         <v>0.85436893199999997</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P45">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
@@ -5603,8 +5779,12 @@
       <c r="O46">
         <v>-0.14459161100000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P46">
+        <f t="shared" si="0"/>
+        <v>1.0000000010000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
@@ -5650,8 +5830,12 @@
       <c r="O47">
         <v>-7.6584506999999996E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P47">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
@@ -5697,8 +5881,12 @@
       <c r="O48">
         <v>-0.83333333300000001</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P48">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
@@ -5744,8 +5932,12 @@
       <c r="O49">
         <v>0.150115473</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
@@ -5791,8 +5983,12 @@
       <c r="O50">
         <v>-1.5037594E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P50">
+        <f t="shared" si="0"/>
+        <v>0.99999999900000014</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
@@ -5838,8 +6034,12 @@
       <c r="O51">
         <v>-0.28021015799999999</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P51">
+        <f t="shared" si="0"/>
+        <v>0.99999999900000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>50</v>
       </c>
@@ -5885,8 +6085,12 @@
       <c r="O52">
         <v>-0.89411764699999996</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P52">
+        <f t="shared" si="0"/>
+        <v>1.0000000010000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
@@ -5932,8 +6136,12 @@
       <c r="O53">
         <v>1.7964072000000001E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P53">
+        <f>C53+D53+E53+F53+G53+H53</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>52</v>
       </c>
@@ -5979,8 +6187,12 @@
       <c r="O54">
         <v>0.13278495900000001</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P54">
+        <f t="shared" si="0"/>
+        <v>1.0000000009999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>
@@ -6026,8 +6238,12 @@
       <c r="O55">
         <v>-0.81818181800000001</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P55">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>54</v>
       </c>
@@ -6073,8 +6289,12 @@
       <c r="O56">
         <v>-0.93506493499999999</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P56">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>55</v>
       </c>
@@ -6120,8 +6340,12 @@
       <c r="O57">
         <v>0.82352941199999996</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P57">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>56</v>
       </c>
@@ -6167,8 +6391,12 @@
       <c r="O58">
         <v>-0.43067846599999998</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P58">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>57</v>
       </c>
@@ -6214,8 +6442,12 @@
       <c r="O59">
         <v>-0.172114402</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P59">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>58</v>
       </c>
@@ -6261,8 +6493,12 @@
       <c r="O60">
         <v>-0.537096774</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P60">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>59</v>
       </c>
@@ -6308,8 +6544,12 @@
       <c r="O61">
         <v>-0.15761821400000001</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P61">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>60</v>
       </c>
@@ -6355,8 +6595,12 @@
       <c r="O62">
         <v>-0.86868686900000003</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P62">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>61</v>
       </c>
@@ -6402,8 +6646,12 @@
       <c r="O63">
         <v>-4.0791099999999997E-2</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P63">
+        <f t="shared" si="0"/>
+        <v>1.0000000010000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>62</v>
       </c>
@@ -6449,8 +6697,12 @@
       <c r="O64">
         <v>-0.243589744</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P64">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>63</v>
       </c>
@@ -6496,8 +6748,12 @@
       <c r="O65">
         <v>0.13318284399999999</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P65">
+        <f t="shared" si="0"/>
+        <v>0.99999999899999992</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>64</v>
       </c>
@@ -6543,8 +6799,12 @@
       <c r="O66">
         <v>8.7531807000000003E-2</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P66">
+        <f t="shared" si="0"/>
+        <v>1.0000000019999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>65</v>
       </c>
@@ -6590,8 +6850,12 @@
       <c r="O67">
         <v>-0.89795918399999997</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P67">
+        <f t="shared" ref="P67:P82" si="1">C67+D67+E67+F67+G67+H67</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>66</v>
       </c>
@@ -6637,8 +6901,12 @@
       <c r="O68">
         <v>-0.756410256</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P68">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>67</v>
       </c>
@@ -6684,8 +6952,12 @@
       <c r="O69">
         <v>-0.45398772999999998</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P69">
+        <f t="shared" si="1"/>
+        <v>0.99999999899999992</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>68</v>
       </c>
@@ -6731,8 +7003,12 @@
       <c r="O70">
         <v>-1</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P70">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>69</v>
       </c>
@@ -6778,8 +7054,12 @@
       <c r="O71">
         <v>-0.13140096600000001</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P71">
+        <f>C71+D71+E71+F71+G71+H71</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>70</v>
       </c>
@@ -6825,8 +7105,12 @@
       <c r="O72">
         <v>-0.86666666699999995</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P72">
+        <f t="shared" si="1"/>
+        <v>0.99999999899999992</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>71</v>
       </c>
@@ -6872,8 +7156,12 @@
       <c r="O73">
         <v>-0.29007633599999999</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P73">
+        <f t="shared" si="1"/>
+        <v>1.0000000010000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>72</v>
       </c>
@@ -6919,8 +7207,12 @@
       <c r="O74">
         <v>0.10227272699999999</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P74">
+        <f t="shared" si="1"/>
+        <v>0.99999999900000003</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>73</v>
       </c>
@@ -6966,8 +7258,12 @@
       <c r="O75">
         <v>0.91071428600000004</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P75">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>74</v>
       </c>
@@ -7013,8 +7309,12 @@
       <c r="O76">
         <v>0.875</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P76">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>75</v>
       </c>
@@ -7060,8 +7360,12 @@
       <c r="O77">
         <v>0.16926069999999999</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P77">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>76</v>
       </c>
@@ -7107,8 +7411,12 @@
       <c r="O78">
         <v>0.28754365500000001</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P78">
+        <f t="shared" si="1"/>
+        <v>0.99999999899999992</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>77</v>
       </c>
@@ -7154,8 +7462,12 @@
       <c r="O79">
         <v>0.13611111100000001</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P79">
+        <f t="shared" si="1"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>78</v>
       </c>
@@ -7201,8 +7513,12 @@
       <c r="O80">
         <v>-0.920903955</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P80">
+        <f t="shared" si="1"/>
+        <v>1.0000000010000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>79</v>
       </c>
@@ -7248,8 +7564,12 @@
       <c r="O81">
         <v>0.813953488</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P81">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>80</v>
       </c>
@@ -7295,8 +7615,12 @@
       <c r="O82">
         <v>0.34444444400000002</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P82">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>81</v>
       </c>
@@ -7342,8 +7666,12 @@
       <c r="O83">
         <v>-1</v>
       </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P83">
+        <f>C83+D83+E83+F83+G83+H83</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>82</v>
       </c>
@@ -7389,8 +7717,12 @@
       <c r="O84">
         <v>-0.25467289700000001</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P84">
+        <f t="shared" ref="P84:P101" si="2">C84+D84+E84+F84+G84+H84</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>83</v>
       </c>
@@ -7436,8 +7768,12 @@
       <c r="O85">
         <v>4.3269230999999998E-2</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P85">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>84</v>
       </c>
@@ -7483,8 +7819,12 @@
       <c r="O86">
         <v>0.40575243999999999</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P86">
+        <f t="shared" si="2"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>85</v>
       </c>
@@ -7530,8 +7870,12 @@
       <c r="O87">
         <v>0.93406593400000004</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P87">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>86</v>
       </c>
@@ -7577,8 +7921,12 @@
       <c r="O88">
         <v>-0.80487804900000004</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P88">
+        <f t="shared" si="2"/>
+        <v>1.0000000010000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>87</v>
       </c>
@@ -7624,8 +7972,12 @@
       <c r="O89">
         <v>-0.495049505</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P89">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>88</v>
       </c>
@@ -7671,8 +8023,12 @@
       <c r="O90">
         <v>-0.42583249200000001</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P90">
+        <f t="shared" si="2"/>
+        <v>1.0000000009999999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>89</v>
       </c>
@@ -7718,8 +8074,12 @@
       <c r="O91">
         <v>0.36200716799999999</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P91">
+        <f t="shared" si="2"/>
+        <v>0.99999999899999981</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>90</v>
       </c>
@@ -7765,8 +8125,12 @@
       <c r="O92">
         <v>-0.32377049200000002</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P92">
+        <f t="shared" si="2"/>
+        <v>1.0000000010000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>91</v>
       </c>
@@ -7812,8 +8176,12 @@
       <c r="O93">
         <v>-0.87288135600000005</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P93">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>92</v>
       </c>
@@ -7859,8 +8227,12 @@
       <c r="O94">
         <v>0.248201439</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P94">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>93</v>
       </c>
@@ -7906,8 +8278,12 @@
       <c r="O95">
         <v>-0.13174404000000001</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P95">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>94</v>
       </c>
@@ -7953,8 +8329,12 @@
       <c r="O96">
         <v>0.94117647100000001</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P96">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>95</v>
       </c>
@@ -8000,8 +8380,12 @@
       <c r="O97">
         <v>-1</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P97">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>96</v>
       </c>
@@ -8047,8 +8431,12 @@
       <c r="O98">
         <v>-0.92241379300000004</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P98">
+        <f t="shared" si="2"/>
+        <v>1.0000000010000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>97</v>
       </c>
@@ -8094,8 +8482,12 @@
       <c r="O99">
         <v>0.91183879099999998</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P99">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>98</v>
       </c>
@@ -8141,8 +8533,12 @@
       <c r="O100">
         <v>-0.68141592900000003</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P100">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>99</v>
       </c>
@@ -8188,8 +8584,12 @@
       <c r="O101">
         <v>-0.79661016900000003</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P101">
+        <f>C101+D101+E101+F101+G101+H101</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>100</v>
       </c>
@@ -8235,8 +8635,12 @@
       <c r="O102">
         <v>-0.24610591900000001</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P102">
+        <f>C102+D102+E102+F102+G102+H102</f>
+        <v>0.99999999899999992</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>101</v>
       </c>
@@ -8282,8 +8686,12 @@
       <c r="O103">
         <v>2.2658610000000001E-3</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P103">
+        <f t="shared" ref="P103:P112" si="3">C103+D103+E103+F103+G103+H103</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>102</v>
       </c>
@@ -8329,8 +8737,12 @@
       <c r="O104">
         <v>0.26268656699999998</v>
       </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P104">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>103</v>
       </c>
@@ -8376,8 +8788,12 @@
       <c r="O105">
         <v>0.34605433400000002</v>
       </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P105">
+        <f t="shared" si="3"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>104</v>
       </c>
@@ -8423,8 +8839,12 @@
       <c r="O106">
         <v>-0.45528455299999998</v>
       </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P106">
+        <f t="shared" si="3"/>
+        <v>0.99999999900000014</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>105</v>
       </c>
@@ -8470,8 +8890,12 @@
       <c r="O107">
         <v>0.101694915</v>
       </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P107">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>106</v>
       </c>
@@ -8517,8 +8941,12 @@
       <c r="O108">
         <v>0.79372197300000003</v>
       </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P108">
+        <f t="shared" si="3"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>107</v>
       </c>
@@ -8564,8 +8992,12 @@
       <c r="O109">
         <v>0.34782608700000001</v>
       </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P109">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>108</v>
       </c>
@@ -8611,8 +9043,12 @@
       <c r="O110">
         <v>0.80672268899999999</v>
       </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P110">
+        <f t="shared" si="3"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>109</v>
       </c>
@@ -8658,8 +9094,12 @@
       <c r="O111">
         <v>-7.5675675999999997E-2</v>
       </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P111">
+        <f t="shared" si="3"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>110</v>
       </c>
@@ -8705,8 +9145,12 @@
       <c r="O112">
         <v>-0.29711576499999998</v>
       </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P112">
+        <f t="shared" si="3"/>
+        <v>1.0000000009999999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>111</v>
       </c>
@@ -8752,8 +9196,12 @@
       <c r="O113">
         <v>-1</v>
       </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P113">
+        <f>C113+D113+E113+F113+G113+H113</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>112</v>
       </c>
@@ -8799,8 +9247,12 @@
       <c r="O114">
         <v>-0.227642276</v>
       </c>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P114">
+        <f t="shared" ref="P114:P116" si="4">C114+D114+E114+F114+G114+H114</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>113</v>
       </c>
@@ -8846,8 +9298,12 @@
       <c r="O115">
         <v>-0.88744588700000004</v>
       </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P115">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>114</v>
       </c>
@@ -8893,8 +9349,12 @@
       <c r="O116">
         <v>0.49272349300000001</v>
       </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P116">
+        <f t="shared" si="4"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>115</v>
       </c>
@@ -8941,7 +9401,7 @@
         <v>2.4759284999999999E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>116</v>
       </c>
@@ -8988,7 +9448,7 @@
         <v>-0.34</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>117</v>
       </c>
@@ -9035,7 +9495,7 @@
         <v>0.89156626500000002</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>118</v>
       </c>
@@ -9082,7 +9542,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>119</v>
       </c>
@@ -9129,7 +9589,7 @@
         <v>-0.60869565199999998</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>120</v>
       </c>
@@ -9176,7 +9636,7 @@
         <v>-0.83333333300000001</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>121</v>
       </c>
@@ -9223,7 +9683,7 @@
         <v>0.24623115600000001</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>122</v>
       </c>
@@ -9270,7 +9730,7 @@
         <v>-0.54875937699999999</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>123</v>
       </c>
@@ -9317,7 +9777,7 @@
         <v>-0.574561404</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>124</v>
       </c>
@@ -9364,7 +9824,7 @@
         <v>0.51219512199999995</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>125</v>
       </c>
@@ -9411,7 +9871,7 @@
         <v>-0.79518072299999998</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>126</v>
       </c>

</xml_diff>